<commit_message>
ER 1932 : Standalone Shipper Management
</commit_message>
<xml_diff>
--- a/desktop/src/ui/vienna_data/data_source.xlsx
+++ b/desktop/src/ui/vienna_data/data_source.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="snmp" sheetId="1" state="visible" r:id="rId2"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="100">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -43,12 +43,18 @@
     <t xml:space="preserve">snmp_device</t>
   </si>
   <si>
+    <t xml:space="preserve">enable_device</t>
+  </si>
+  <si>
     <t xml:space="preserve">credential</t>
   </si>
   <si>
     <t xml:space="preserve">snmp_timeout</t>
   </si>
   <si>
+    <t xml:space="preserve">standalone_shipper</t>
+  </si>
+  <si>
     <t xml:space="preserve">mib_groups.interval:mib_group</t>
   </si>
   <si>
@@ -64,9 +70,15 @@
     <t xml:space="preserve">CiscoIos</t>
   </si>
   <si>
+    <t xml:space="preserve">No</t>
+  </si>
+  <si>
     <t xml:space="preserve">first</t>
   </si>
   <si>
+    <t xml:space="preserve">127.0.0.1</t>
+  </si>
+  <si>
     <t xml:space="preserve">360:INTERFACE_MIB_GROUP</t>
   </si>
   <si>
@@ -112,9 +124,6 @@
     <t xml:space="preserve">My Network Elements 1</t>
   </si>
   <si>
-    <t xml:space="preserve">No</t>
-  </si>
-  <si>
     <t xml:space="preserve">12.12.12.1</t>
   </si>
   <si>
@@ -284,6 +293,9 @@
   </si>
   <si>
     <t xml:space="preserve">configuration_collector_target</t>
+  </si>
+  <si>
+    <t xml:space="preserve">interval</t>
   </si>
   <si>
     <t xml:space="preserve">configuration_collector_vendor</t>
@@ -452,28 +464,32 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H:H"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.4336734693878"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="20.25"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="27.5408163265306"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="28.6173469387755"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="30.2397959183673"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="23.3520408163265"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="26.8622448979592"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="29.4285714285714"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -498,37 +514,49 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
-      <c r="P1" s="2"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="G2" s="0" t="s">
-        <v>12</v>
+      <c r="H2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -550,22 +578,23 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
+      <selection pane="topLeft" activeCell="K1" activeCellId="1" sqref="H:H K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="22.0051020408163"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="32.6683673469388"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="31.8571428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -573,54 +602,54 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>5065</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>300</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="G2" s="0" t="n">
         <v>3</v>
@@ -635,7 +664,7 @@
         <v>2000</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -657,43 +686,47 @@
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="1" sqref="H:H F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.85"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.4336734693878"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.25"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="27.5408163265306"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="28.6173469387755"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="30.2397959183673"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="23.3520408163265"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="26.8622448979592"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="29.4285714285714"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1"/>
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -704,21 +737,24 @@
       <c r="N1" s="1"/>
       <c r="O1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -740,20 +776,21 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+      <selection pane="topLeft" activeCell="C13" activeCellId="1" sqref="H:H C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="32.6683673469388"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="31.8571428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -761,39 +798,39 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>5060</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>300</v>
@@ -811,18 +848,18 @@
         <v>3000</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>5060</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>300</v>
@@ -840,18 +877,18 @@
         <v>3000</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B4" s="4" t="n">
         <v>5060</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="D4" s="4" t="n">
         <v>300</v>
@@ -869,7 +906,7 @@
         <v>3000</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -882,7 +919,7 @@
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
       <c r="I5" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -914,18 +951,20 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H:H"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="44.9540816326531"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="43.8724489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -933,39 +972,39 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>5070</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>300</v>
@@ -983,18 +1022,18 @@
         <v>8000</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>5070</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>300</v>
@@ -1012,18 +1051,18 @@
         <v>8000</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B4" s="4" t="n">
         <v>5070</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="D4" s="4" t="n">
         <v>300</v>
@@ -1041,7 +1080,7 @@
         <v>8000</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1056,7 +1095,7 @@
         <v>8000</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1087,17 +1126,17 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="H:H E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="32.8010204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.9948979591837"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1105,30 +1144,30 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>5085</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>300</v>
@@ -1137,18 +1176,18 @@
         <v>30000</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>5085</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>300</v>
@@ -1157,18 +1196,18 @@
         <v>30000</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B4" s="4" t="n">
         <v>5085</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="D4" s="4" t="n">
         <v>300</v>
@@ -1177,7 +1216,7 @@
         <v>30000</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1187,7 +1226,7 @@
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="5" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1221,15 +1260,17 @@
   <dimension ref="1:2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P1" activeCellId="0" sqref="P1"/>
+      <selection pane="topLeft" activeCell="P1" activeCellId="1" sqref="H:H P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="15" min="6" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="22.8112244897959"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="5" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="15" min="6" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="36.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1237,107 +1278,107 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="P1" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="AMI1" s="0"/>
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>5006</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="F2" s="3" t="n">
         <v>300</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="O2" s="0" t="n">
         <v>200</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="Q2" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1363,13 +1404,15 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="1" sqref="H:H D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.5816326530612"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.6377551020408"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1377,33 +1420,33 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="D1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>5080</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>5080</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1425,12 +1468,12 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="1" sqref="H:H C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="3" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="3" width="9.04591836734694"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1438,27 +1481,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B2" s="3" t="n">
         <v>5009</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1477,39 +1520,45 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="1" sqref="H:H G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.85"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.6785714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.4897959183673"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.4336734693878"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="23.0816326530612"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.8112244897959"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.0816326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+        <v>90</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -1517,23 +1566,30 @@
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
-      <c r="O1" s="2"/>
-    </row>
-    <row r="2" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O1" s="1"/>
+      <c r="P1" s="2"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>9</v>
+        <v>21</v>
+      </c>
+      <c r="C2" s="3" t="n">
+        <v>360</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="0" t="s">
         <v>11</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ER-2213 : replaced data_source.xlsx file with latest one (#139)
</commit_message>
<xml_diff>
--- a/desktop/src/ui/vienna_data/data_source.xlsx
+++ b/desktop/src/ui/vienna_data/data_source.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="snmp" sheetId="1" state="visible" r:id="rId2"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="100">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -466,30 +466,28 @@
   </sheetPr>
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H:H"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="29.4285714285714"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="22.6785714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="28.6173469387755"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="22.1377551020408"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -575,26 +573,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K1" activeCellId="1" sqref="H:H K1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9285714285714"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="26.0510204081633"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="31.8571428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.0816326530612"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="31.0459183673469"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -608,27 +605,30 @@
         <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>99</v>
       </c>
     </row>
@@ -642,28 +642,31 @@
       <c r="C2" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="0" t="n">
         <v>300</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="G2" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="H2" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="H2" s="3" t="n">
+      <c r="I2" s="3" t="n">
         <v>30000</v>
       </c>
-      <c r="I2" s="0" t="n">
+      <c r="J2" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="J2" s="0" t="n">
+      <c r="K2" s="0" t="n">
         <v>2000</v>
       </c>
-      <c r="K2" s="0" t="s">
+      <c r="L2" s="0" t="s">
         <v>31</v>
       </c>
     </row>
@@ -686,26 +689,24 @@
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="1" sqref="H:H F1"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="29.4285714285714"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="22.6785714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="28.6173469387755"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="22.1377551020408"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -773,24 +774,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="1" sqref="H:H C13"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9285714285714"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="24.3010204081633"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="31.8571428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="31.0459183673469"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -804,21 +804,24 @@
         <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>29</v>
       </c>
     </row>
@@ -832,22 +835,25 @@
       <c r="C2" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="0" t="n">
         <v>300</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="F2" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="G2" s="0" t="n">
         <v>500</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="H2" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="H2" s="0" t="n">
+      <c r="I2" s="0" t="n">
         <v>3000</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="J2" s="0" t="s">
         <v>31</v>
       </c>
     </row>
@@ -861,22 +867,25 @@
       <c r="C3" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="0" t="n">
         <v>300</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="F3" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="G3" s="0" t="n">
         <v>500</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="H3" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="H3" s="0" t="n">
+      <c r="I3" s="0" t="n">
         <v>3000</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>21</v>
       </c>
     </row>
@@ -890,22 +899,25 @@
       <c r="C4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="4" t="n">
+      <c r="D4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="4" t="n">
         <v>300</v>
       </c>
-      <c r="E4" s="4" t="n">
+      <c r="F4" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="F4" s="4" t="n">
+      <c r="G4" s="4" t="n">
         <v>500</v>
       </c>
-      <c r="G4" s="4" t="n">
+      <c r="H4" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="H4" s="4" t="n">
+      <c r="I4" s="4" t="n">
         <v>3000</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>34</v>
       </c>
     </row>
@@ -918,8 +930,197 @@
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
-      <c r="I5" s="3" t="s">
+      <c r="I5" s="4"/>
+      <c r="J5" s="3" t="s">
         <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="I4:I5"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:J5"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="23.0816326530612"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="42.7908163265306"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>5070</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>5070</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="4" t="n">
+        <v>5070</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="4" t="n">
+        <v>300</v>
+      </c>
+      <c r="F4" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="G4" s="4" t="n">
+        <v>500</v>
+      </c>
+      <c r="H4" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -943,28 +1144,25 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H:H"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="43.8724489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="3.51020408163265"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.1836734693878"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -978,109 +1176,85 @@
         <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>5070</v>
+        <v>5085</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="0" t="n">
         <v>300</v>
       </c>
-      <c r="E2" s="0" t="n">
-        <v>3</v>
-      </c>
       <c r="F2" s="0" t="n">
-        <v>500</v>
-      </c>
-      <c r="G2" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="H2" s="0" t="n">
-        <v>8000</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>43</v>
+        <v>30000</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>5070</v>
+        <v>5085</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="0" t="n">
         <v>300</v>
       </c>
-      <c r="E3" s="0" t="n">
-        <v>3</v>
-      </c>
       <c r="F3" s="0" t="n">
-        <v>500</v>
-      </c>
-      <c r="G3" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="H3" s="0" t="n">
-        <v>8000</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>45</v>
+        <v>30000</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="B4" s="4" t="n">
-        <v>5070</v>
+        <v>5085</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="4" t="n">
+      <c r="D4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="4" t="n">
         <v>300</v>
       </c>
-      <c r="E4" s="4" t="n">
-        <v>3</v>
-      </c>
       <c r="F4" s="4" t="n">
-        <v>500</v>
-      </c>
-      <c r="G4" s="4" t="n">
-        <v>20</v>
-      </c>
-      <c r="H4" s="0" t="n">
-        <v>8000</v>
-      </c>
-      <c r="I4" s="0" t="s">
-        <v>47</v>
+        <v>30000</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1090,157 +1264,23 @@
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="0" t="n">
-        <v>8000</v>
-      </c>
-      <c r="I5" s="0" t="s">
-        <v>48</v>
+      <c r="G5" s="5" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="6">
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="F4:F5"/>
-    <mergeCell ref="G4:G5"/>
-  </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:F5"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="H:H E1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.3010204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.9948979591837"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <v>5085</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>300</v>
-      </c>
-      <c r="E2" s="0" t="n">
-        <v>30000</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>5085</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>300</v>
-      </c>
-      <c r="E3" s="0" t="n">
-        <v>30000</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B4" s="4" t="n">
-        <v>5085</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="4" t="n">
-        <v>300</v>
-      </c>
-      <c r="E4" s="4" t="n">
-        <v>30000</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" display="http://12.12.12.1/index.html"/>
-    <hyperlink ref="F3" r:id="rId2" display="http://google.co.in"/>
-    <hyperlink ref="F5" r:id="rId3" display="https://164.164.37.9/vunet.html"/>
+    <hyperlink ref="G2" r:id="rId1" display="http://12.12.12.1/index.html"/>
+    <hyperlink ref="G3" r:id="rId2" display="http://google.co.in"/>
+    <hyperlink ref="G5" r:id="rId3" display="https://164.164.37.9/vunet.html"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1260,17 +1300,15 @@
   <dimension ref="1:2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P1" activeCellId="1" sqref="H:H P1"/>
+      <selection pane="topLeft" activeCell="P1" activeCellId="0" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="2" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="15" min="6" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="15" min="6" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="21.734693877551"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="36.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1404,15 +1442,13 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="1" sqref="H:H D3"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.6377551020408"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.6938775510204"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1468,12 +1504,12 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="1" sqref="H:H C7"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="3" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="3" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1523,18 +1559,17 @@
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="1" sqref="H:H G1"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="23.0816326530612"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.8112244897959"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.0816326530612"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="22.5459183673469"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.5459183673469"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>